<commit_message>
Final change outreach sent
</commit_message>
<xml_diff>
--- a/resources/Companies to contact.xlsx
+++ b/resources/Companies to contact.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="116">
   <si>
     <t>Company</t>
   </si>
@@ -40,6 +40,15 @@
     <t>Notes:</t>
   </si>
   <si>
+    <t>Unnamed: 8</t>
+  </si>
+  <si>
+    <t>Unnamed: 9</t>
+  </si>
+  <si>
+    <t>Unnamed: 10</t>
+  </si>
+  <si>
     <t>Military Support Foundation</t>
   </si>
   <si>
@@ -49,6 +58,9 @@
     <t xml:space="preserve">Price </t>
   </si>
   <si>
+    <t>Sent</t>
+  </si>
+  <si>
     <t>Reyness@militarysupport.net</t>
   </si>
   <si>
@@ -65,9 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">Knutson </t>
-  </si>
-  <si>
-    <t>Sent</t>
   </si>
   <si>
     <t>keith.knutson@honeywell.com</t>
@@ -359,8 +368,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd hh:mm:ss"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,16 +386,9 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -396,12 +400,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -415,48 +434,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -484,28 +482,28 @@
         <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="145F82"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E87331"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="186C24"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -767,17 +765,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="35.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="23.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="25.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="36.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="20.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
@@ -805,610 +803,634 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="6" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2">
-        <v>45568</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
+      <c r="E3" s="5">
+        <v>25568.708860740742</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="3"/>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>25</v>
+      <c r="F4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>28</v>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="3"/>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>34</v>
+      <c r="F6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+      <c r="A7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>37</v>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+      <c r="A8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="1" t="s">
-        <v>39</v>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="3"/>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+      <c r="A9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>45</v>
+      <c r="F9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="3"/>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+      <c r="A10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>49</v>
+      <c r="F10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+      <c r="A11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>52</v>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+      <c r="A12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>55</v>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="8">
-      <c r="A13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="3"/>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+      <c r="A13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+      <c r="A14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" s="7"/>
+      <c r="F14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+      <c r="A15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="1" t="s">
-        <v>60</v>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
+      <c r="A16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="1" t="s">
-        <v>62</v>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+      <c r="A17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="1" t="s">
-        <v>64</v>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="3"/>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+      <c r="A18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G18" s="7"/>
+      <c r="F18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="3"/>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+      <c r="A19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="1" t="s">
-        <v>69</v>
+      <c r="F19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+      <c r="A20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="1" t="s">
-        <v>71</v>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
+      <c r="A21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="1" t="s">
-        <v>73</v>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="33" customFormat="1" s="8">
-      <c r="A22" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+      <c r="A22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
+      <c r="A23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="1" t="s">
-        <v>76</v>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
-      <c r="A24" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="A24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="1" t="s">
-        <v>78</v>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
-      <c r="A25" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
+      <c r="A25" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="1" t="s">
-        <v>80</v>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="1" t="s">
-        <v>81</v>
+      <c r="K25" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
-      <c r="A26" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
+      <c r="A26" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="1" t="s">
-        <v>83</v>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
-      <c r="A27" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+      <c r="A27" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>86</v>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
-      <c r="A28" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+      <c r="A28" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="1" t="s">
-        <v>88</v>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18">
-      <c r="A29" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
+      <c r="A29" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="1" t="s">
-        <v>90</v>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
-      <c r="A30" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+      <c r="A30" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="1" t="s">
-        <v>92</v>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="1" t="s">
-        <v>93</v>
+      <c r="K30" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18">
-      <c r="A31" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="A31" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="1" t="s">
-        <v>95</v>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18">
-      <c r="A32" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+      <c r="A32" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>98</v>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
-      <c r="A33" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="3"/>
+      <c r="A33" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>101</v>
+      <c r="F33" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -1416,86 +1438,88 @@
       <c r="K33" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
-      <c r="A34" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
+      <c r="A34" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="1" t="s">
-        <v>103</v>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18" customFormat="1" s="8">
-      <c r="A35" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18" customFormat="1" s="8">
-      <c r="A36" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
+      <c r="A35" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
+      <c r="A36" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
-      <c r="A37" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
+      <c r="A37" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="4"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="1" t="s">
-        <v>107</v>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
-      <c r="A38" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D38" s="3"/>
+      <c r="A38" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E38" s="4"/>
-      <c r="F38" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>112</v>
+      <c r="F38" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>

</xml_diff>